<commit_message>
Processed Results - nexus 5x completed
</commit_message>
<xml_diff>
--- a/Processed Results/Nexus 5X/Room Database/Room Database - Processed.xlsx
+++ b/Processed Results/Nexus 5X/Room Database/Room Database - Processed.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\Room Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Nexus 5X\Room Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA48928-5EE2-4352-AA4B-C8FA6121166F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FA064B-0A66-43FD-9F6D-B8E4E0CE53FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="100" windowWidth="9990" windowHeight="7360" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
+    <workbookView xWindow="130" yWindow="120" windowWidth="9990" windowHeight="9830" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$98:$A$187</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$98:$B$187</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$2:$A$31</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$2:$B$31</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Blad1!$A$98:$A$187</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Blad1!$B$98:$B$187</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$2:$A$31</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$2:$B$31</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$A$34:$A$63</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$B$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$34:$B$63</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$A$66:$A$95</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$B$65</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$66:$B$95</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$34:$A$63</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$33</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$B$34:$B$63</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$A$66:$A$95</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$65</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$B$66:$B$95</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$A$98:$A$187</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$98:$B$187</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -285,94 +285,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>95.335919999999902</c:v>
+                  <c:v>111.14243999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.437159999999906</c:v>
+                  <c:v>127.04219999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.965199999999996</c:v>
+                  <c:v>128.13336000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.335919999999902</c:v>
+                  <c:v>127.35396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.279839999999993</c:v>
+                  <c:v>127.50984</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.807879999999997</c:v>
+                  <c:v>127.50984</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95.965199999999996</c:v>
+                  <c:v>126.574559999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.021280000000004</c:v>
+                  <c:v>127.50984</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>96.279839999999993</c:v>
+                  <c:v>126.88632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>94.863960000000006</c:v>
+                  <c:v>122.36579999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94.549319999999994</c:v>
+                  <c:v>127.8216</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95.807879999999997</c:v>
+                  <c:v>127.19808</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>95.49324</c:v>
+                  <c:v>126.73044</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>95.178600000000003</c:v>
+                  <c:v>127.04219999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>95.49324</c:v>
+                  <c:v>127.35396</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>95.807879999999997</c:v>
+                  <c:v>126.418679999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>94.234679999999997</c:v>
+                  <c:v>127.19808</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>95.178600000000003</c:v>
+                  <c:v>127.04219999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>95.49324</c:v>
+                  <c:v>127.04219999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95.021280000000004</c:v>
+                  <c:v>127.04219999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>95.335919999999902</c:v>
+                  <c:v>127.19808</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>95.021280000000004</c:v>
+                  <c:v>127.97748</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>97.538399999999996</c:v>
+                  <c:v>127.04219999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>95.335919999999902</c:v>
+                  <c:v>126.88632</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>95.807879999999997</c:v>
+                  <c:v>127.35396</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>95.178600000000003</c:v>
+                  <c:v>127.19808</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>95.178600000000003</c:v>
+                  <c:v>121.898159999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>95.335919999999902</c:v>
+                  <c:v>126.73044</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>95.335919999999902</c:v>
+                  <c:v>127.35396</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>95.49324</c:v>
+                  <c:v>127.19808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,10 +456,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>95.503727999999981</c:v>
+                  <c:v>126.32515199999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95.503727999999981</c:v>
+                  <c:v>126.32515199999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,94 +920,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>98.027315999999999</c:v>
+                  <c:v>113.247828</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99.452591999999996</c:v>
+                  <c:v>132.04414800000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.502407999999903</c:v>
+                  <c:v>115.91064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.185680000000005</c:v>
+                  <c:v>116.067275999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.027315999999999</c:v>
+                  <c:v>133.92377999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.810220000000001</c:v>
+                  <c:v>111.838104</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.344043999999997</c:v>
+                  <c:v>116.067275999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>97.235495999999898</c:v>
+                  <c:v>116.067275999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>96.918768</c:v>
+                  <c:v>116.537184</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>97.393860000000004</c:v>
+                  <c:v>133.45387199999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>97.393860000000004</c:v>
+                  <c:v>116.380547999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.760403999999994</c:v>
+                  <c:v>115.440732</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98.502407999999903</c:v>
+                  <c:v>133.297236</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>98.819136</c:v>
+                  <c:v>133.297236</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97.552223999999995</c:v>
+                  <c:v>133.76714399999901</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>96.760403999999994</c:v>
+                  <c:v>116.067275999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>96.918768</c:v>
+                  <c:v>114.97082399999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>96.285312000000005</c:v>
+                  <c:v>115.28409600000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>97.393860000000004</c:v>
+                  <c:v>115.597368</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>97.235495999999898</c:v>
+                  <c:v>118.260179999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>97.077131999999906</c:v>
+                  <c:v>130.94769600000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>97.552223999999995</c:v>
+                  <c:v>131.73087599999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>99.135863999999998</c:v>
+                  <c:v>124.99552799999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>97.552223999999995</c:v>
+                  <c:v>132.35741999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>96.918768</c:v>
+                  <c:v>131.41760399999899</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>98.185680000000005</c:v>
+                  <c:v>131.26096799999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>96.918768</c:v>
+                  <c:v>131.57424</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>96.443675999999996</c:v>
+                  <c:v>131.41760399999899</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>98.977500000000006</c:v>
+                  <c:v>131.88751199999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>96.760403999999994</c:v>
+                  <c:v>134.863596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,10 +1059,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>97.568060399999979</c:v>
+                  <c:v>124.33243559999967</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.568060399999979</c:v>
+                  <c:v>124.33243559999967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,6 +1206,7 @@
         <c:axId val="489458320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="110"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1614,94 +1615,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>97.655471999999904</c:v>
+                  <c:v>113.5611</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.768807999999893</c:v>
+                  <c:v>129.537972</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.405000000000001</c:v>
+                  <c:v>111.211559999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.882143999999997</c:v>
+                  <c:v>128.911428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.723095999999899</c:v>
+                  <c:v>111.211559999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.655471999999904</c:v>
+                  <c:v>128.911428</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.927855999999906</c:v>
+                  <c:v>128.911428</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98.768807999999893</c:v>
+                  <c:v>129.22469999999899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>99.245952000000003</c:v>
+                  <c:v>129.06806399999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>97.337375999999907</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>97.655471999999904</c:v>
+                  <c:v>129.85124399999901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>98.609759999999994</c:v>
+                  <c:v>128.28488399999901</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>97.655471999999904</c:v>
+                  <c:v>129.06806399999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>97.496424000000005</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>98.768807999999893</c:v>
+                  <c:v>129.06806399999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>98.132615999999999</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>98.927855999999906</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>98.450711999999996</c:v>
+                  <c:v>129.06806399999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>97.973568</c:v>
+                  <c:v>129.06806399999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>97.337375999999907</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>97.814520000000002</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>98.291663999999997</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>97.019279999999995</c:v>
+                  <c:v>124.99552799999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>98.768807999999893</c:v>
+                  <c:v>129.22469999999899</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>97.178327999999993</c:v>
+                  <c:v>128.911428</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>98.132615999999999</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>98.291663999999997</c:v>
+                  <c:v>129.381336</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>99.086904000000004</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>96.224039999999903</c:v>
+                  <c:v>128.911428</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>98.132615999999999</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,10 +1754,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>98.243949599999937</c:v>
+                  <c:v>127.11011399999981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.243949599999937</c:v>
+                  <c:v>127.11011399999981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,10 +2102,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2180,7 +2181,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="98" min="94"/>
+        <cx:valScaling min="110"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2223,10 +2224,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2301,7 +2302,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling min="110"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2344,10 +2345,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2385,7 +2386,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3F5A16A3-6E4C-4475-A634-1322A70DC713}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>Medium_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2429,7 +2430,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="100" min="95.5"/>
+        <cx:valScaling min="110"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2472,10 +2473,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2513,7 +2514,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{138ACD3C-CAEA-4AEF-B3DF-B982F1EA92CC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>High_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2557,7 +2558,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="100.5" min="96"/>
+        <cx:valScaling min="110"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -7207,8 +7208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FE0459-F6C0-45BE-AD60-56F63431C3F0}">
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B185" activeCellId="2" sqref="B187 B186 B98:B185"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B99" activeCellId="1" sqref="B98 B99:B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7231,7 +7232,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>95.335919999999902</v>
+        <v>111.14243999999999</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
@@ -7245,14 +7246,14 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>96.437159999999906</v>
+        <v>127.04219999999999</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>95.503727999999981</v>
+        <v>126.32515199999989</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -7260,14 +7261,14 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>95.965199999999996</v>
+        <v>128.13336000000001</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>95.503727999999981</v>
+        <v>126.32515199999989</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -7275,7 +7276,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>95.335919999999902</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -7283,7 +7284,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>96.279839999999993</v>
+        <v>127.50984</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -7297,15 +7298,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>95.807879999999997</v>
+        <v>127.50984</v>
       </c>
       <c r="D7" s="1">
         <f>MIN(B2:B31)</f>
-        <v>94.234679999999997</v>
+        <v>111.14243999999999</v>
       </c>
       <c r="E7" s="1">
         <f>MAX(B2:B31)</f>
-        <v>97.538399999999996</v>
+        <v>128.13336000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -7313,7 +7314,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>95.965199999999996</v>
+        <v>126.574559999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -7321,7 +7322,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>95.021280000000004</v>
+        <v>127.50984</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
@@ -7335,15 +7336,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>96.279839999999993</v>
+        <v>126.88632</v>
       </c>
       <c r="D10">
         <f>QUARTILE(B2:B31, 1)</f>
-        <v>95.178600000000003</v>
+        <v>126.88632</v>
       </c>
       <c r="E10">
         <f>QUARTILE(B2:B31, 2)</f>
-        <v>95.335919999999902</v>
+        <v>127.12013999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -7351,7 +7352,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>94.863960000000006</v>
+        <v>122.36579999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -7359,7 +7360,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>94.549319999999994</v>
+        <v>127.8216</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -7373,15 +7374,15 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>95.807879999999997</v>
+        <v>127.19808</v>
       </c>
       <c r="D13">
         <f>QUARTILE(B2:B31, 3)</f>
-        <v>95.807879999999997</v>
+        <v>127.35396</v>
       </c>
       <c r="E13">
         <f xml:space="preserve"> D13 - D10</f>
-        <v>0.62927999999999429</v>
+        <v>0.46764000000000294</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -7389,7 +7390,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>95.49324</v>
+        <v>126.73044</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -7397,7 +7398,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>95.178600000000003</v>
+        <v>127.04219999999999</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -7411,15 +7412,15 @@
         <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>95.49324</v>
+        <v>127.35396</v>
       </c>
       <c r="D16">
         <f>STDEV(B2:B31)</f>
-        <v>0.62237061985438358</v>
+        <v>3.1644421111474066</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (D16 / E4) * 100</f>
-        <v>0.65167154506720792</v>
+        <v>2.5049976675645791</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -7427,7 +7428,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>95.807879999999997</v>
+        <v>126.418679999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -7435,7 +7436,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="1">
-        <v>94.234679999999997</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -7443,7 +7444,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="1">
-        <v>95.178600000000003</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7451,7 +7452,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>95.49324</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -7459,7 +7460,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="1">
-        <v>95.021280000000004</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -7467,7 +7468,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1">
-        <v>95.335919999999902</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -7475,7 +7476,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="1">
-        <v>95.021280000000004</v>
+        <v>127.97748</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -7483,7 +7484,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1">
-        <v>97.538399999999996</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -7491,7 +7492,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>95.335919999999902</v>
+        <v>126.88632</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -7499,7 +7500,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="1">
-        <v>95.807879999999997</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -7507,7 +7508,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="1">
-        <v>95.178600000000003</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -7515,7 +7516,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="1">
-        <v>95.178600000000003</v>
+        <v>121.898159999999</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -7523,7 +7524,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="1">
-        <v>95.335919999999902</v>
+        <v>126.73044</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -7531,7 +7532,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1">
-        <v>95.335919999999902</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -7539,7 +7540,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="1">
-        <v>95.49324</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -7558,7 +7559,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="1">
-        <v>98.027315999999999</v>
+        <v>113.247828</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -7572,14 +7573,14 @@
         <v>12</v>
       </c>
       <c r="B35" s="1">
-        <v>99.452591999999996</v>
+        <v>132.04414800000001</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" s="1">
         <f>AVERAGE(B34,B35,B36,B37,B38,B39,B40,B41,B42,B43,B44,B45,B46,B47,B48,B49,B50,B51,B53,B52,B54,B55,B56,B57,B58,B59,B60,B61,B62,B63)</f>
-        <v>97.568060399999979</v>
+        <v>124.33243559999967</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -7587,14 +7588,14 @@
         <v>12</v>
       </c>
       <c r="B36" s="1">
-        <v>98.502407999999903</v>
+        <v>115.91064</v>
       </c>
       <c r="D36">
         <v>30</v>
       </c>
       <c r="E36" s="1">
         <f>AVERAGE(B34,B35,B36,B37,B38,B39,B40,B41,B42,B43,B44,B45,B46,B47,B48,B49,B50,B51,B53,B52,B54,B55,B56,B57,B58,B59,B60,B61,B62,B63)</f>
-        <v>97.568060399999979</v>
+        <v>124.33243559999967</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -7602,7 +7603,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="1">
-        <v>98.185680000000005</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -7610,7 +7611,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="1">
-        <v>98.027315999999999</v>
+        <v>133.92377999999999</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>3</v>
@@ -7624,15 +7625,15 @@
         <v>12</v>
       </c>
       <c r="B39" s="1">
-        <v>95.810220000000001</v>
+        <v>111.838104</v>
       </c>
       <c r="D39" s="1">
         <f>MIN(B34:B63)</f>
-        <v>95.810220000000001</v>
+        <v>111.838104</v>
       </c>
       <c r="E39" s="1">
         <f>MAX(B34:B63)</f>
-        <v>99.452591999999996</v>
+        <v>134.863596</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -7640,7 +7641,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="1">
-        <v>98.344043999999997</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -7648,7 +7649,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="1">
-        <v>97.235495999999898</v>
+        <v>116.067275999999</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>5</v>
@@ -7662,15 +7663,15 @@
         <v>12</v>
       </c>
       <c r="B42" s="1">
-        <v>96.918768</v>
+        <v>116.537184</v>
       </c>
       <c r="D42">
         <f>QUARTILE(B34:B63, 1)</f>
-        <v>96.918768</v>
+        <v>116.067275999999</v>
       </c>
       <c r="E42">
         <f>QUARTILE(B34:B63, 2)</f>
-        <v>97.393860000000004</v>
+        <v>127.97161199999999</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -7678,7 +7679,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="1">
-        <v>97.393860000000004</v>
+        <v>133.45387199999999</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -7686,7 +7687,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="1">
-        <v>97.393860000000004</v>
+        <v>116.380547999999</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -7700,15 +7701,15 @@
         <v>12</v>
       </c>
       <c r="B45" s="1">
-        <v>96.760403999999994</v>
+        <v>115.440732</v>
       </c>
       <c r="D45">
         <f>QUARTILE(B34:B63, 3)</f>
-        <v>98.185680000000005</v>
+        <v>132.00498899999999</v>
       </c>
       <c r="E45">
         <f xml:space="preserve"> D45 - D42</f>
-        <v>1.2669120000000049</v>
+        <v>15.937713000000997</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -7716,7 +7717,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="1">
-        <v>98.502407999999903</v>
+        <v>133.297236</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -7724,7 +7725,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="1">
-        <v>98.819136</v>
+        <v>133.297236</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>16</v>
@@ -7738,15 +7739,15 @@
         <v>12</v>
       </c>
       <c r="B48" s="1">
-        <v>97.552223999999995</v>
+        <v>133.76714399999901</v>
       </c>
       <c r="D48">
         <f>STDEV(B34:B63)</f>
-        <v>0.89617987414463807</v>
+        <v>8.5611117884821191</v>
       </c>
       <c r="E48">
         <f xml:space="preserve"> (D48 / E36) * 100</f>
-        <v>0.91851766907179222</v>
+        <v>6.8856624155781772</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -7754,7 +7755,7 @@
         <v>12</v>
       </c>
       <c r="B49" s="1">
-        <v>96.760403999999994</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -7762,7 +7763,7 @@
         <v>12</v>
       </c>
       <c r="B50" s="1">
-        <v>96.918768</v>
+        <v>114.97082399999999</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -7770,7 +7771,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="1">
-        <v>96.285312000000005</v>
+        <v>115.28409600000001</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -7778,7 +7779,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="1">
-        <v>97.393860000000004</v>
+        <v>115.597368</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -7786,7 +7787,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="1">
-        <v>97.235495999999898</v>
+        <v>118.260179999999</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -7794,7 +7795,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="1">
-        <v>97.077131999999906</v>
+        <v>130.94769600000001</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -7802,7 +7803,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="1">
-        <v>97.552223999999995</v>
+        <v>131.73087599999999</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -7810,7 +7811,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="1">
-        <v>99.135863999999998</v>
+        <v>124.99552799999999</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -7818,7 +7819,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="1">
-        <v>97.552223999999995</v>
+        <v>132.35741999999999</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -7826,7 +7827,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1">
-        <v>96.918768</v>
+        <v>131.41760399999899</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -7834,7 +7835,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="1">
-        <v>98.185680000000005</v>
+        <v>131.26096799999999</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -7842,7 +7843,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="1">
-        <v>96.918768</v>
+        <v>131.57424</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -7850,7 +7851,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="1">
-        <v>96.443675999999996</v>
+        <v>131.41760399999899</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -7858,7 +7859,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="1">
-        <v>98.977500000000006</v>
+        <v>131.88751199999999</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -7866,7 +7867,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="1">
-        <v>96.760403999999994</v>
+        <v>134.863596</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -7885,7 +7886,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="1">
-        <v>97.655471999999904</v>
+        <v>113.5611</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
@@ -7899,14 +7900,14 @@
         <v>14</v>
       </c>
       <c r="B67" s="1">
-        <v>98.768807999999893</v>
+        <v>129.537972</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67" s="1">
         <f>AVERAGE(B66,B67,B68,B69,B70,B71,B72,B73,B74,B75,B76,B77,B78,B79,B80,B81,B82,B83,B85,B84,B86,B87,B88,B89,B90,B91,B92,B93,B94,B95)</f>
-        <v>98.243949599999937</v>
+        <v>127.11011399999981</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -7914,14 +7915,14 @@
         <v>14</v>
       </c>
       <c r="B68" s="1">
-        <v>99.405000000000001</v>
+        <v>111.211559999999</v>
       </c>
       <c r="D68">
         <v>30</v>
       </c>
       <c r="E68" s="1">
         <f>AVERAGE(B66,B67,B68,B69,B70,B71,B72,B73,B74,B75,B76,B77,B78,B79,B80,B81,B82,B83,B85,B84,B86,B87,B88,B89,B90,B91,B92,B93,B94,B95)</f>
-        <v>98.243949599999937</v>
+        <v>127.11011399999981</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -7929,7 +7930,7 @@
         <v>14</v>
       </c>
       <c r="B69" s="1">
-        <v>99.882143999999997</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -7937,7 +7938,7 @@
         <v>14</v>
       </c>
       <c r="B70" s="1">
-        <v>99.723095999999899</v>
+        <v>111.211559999999</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>3</v>
@@ -7951,15 +7952,15 @@
         <v>14</v>
       </c>
       <c r="B71" s="1">
-        <v>97.655471999999904</v>
+        <v>128.911428</v>
       </c>
       <c r="D71" s="1">
         <f>MIN(B66:B95)</f>
-        <v>96.224039999999903</v>
+        <v>111.211559999999</v>
       </c>
       <c r="E71" s="1">
         <f>MAX(B66:B95)</f>
-        <v>99.882143999999997</v>
+        <v>129.85124399999901</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -7967,7 +7968,7 @@
         <v>14</v>
       </c>
       <c r="B72" s="1">
-        <v>98.927855999999906</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -7975,7 +7976,7 @@
         <v>14</v>
       </c>
       <c r="B73" s="1">
-        <v>98.768807999999893</v>
+        <v>129.22469999999899</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>5</v>
@@ -7989,15 +7990,15 @@
         <v>14</v>
       </c>
       <c r="B74" s="1">
-        <v>99.245952000000003</v>
+        <v>129.06806399999999</v>
       </c>
       <c r="D74">
         <f>QUARTILE(B66:B95, 1)</f>
-        <v>97.655471999999904</v>
+        <v>128.59815599999999</v>
       </c>
       <c r="E74">
         <f>QUARTILE(B66:B95, 2)</f>
-        <v>98.212140000000005</v>
+        <v>128.83311</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -8005,7 +8006,7 @@
         <v>14</v>
       </c>
       <c r="B75" s="1">
-        <v>97.337375999999907</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -8013,7 +8014,7 @@
         <v>14</v>
       </c>
       <c r="B76" s="1">
-        <v>97.655471999999904</v>
+        <v>129.85124399999901</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
@@ -8027,15 +8028,15 @@
         <v>14</v>
       </c>
       <c r="B77" s="1">
-        <v>98.609759999999994</v>
+        <v>128.28488399999901</v>
       </c>
       <c r="D77">
         <f>QUARTILE(B66:B95, 3)</f>
-        <v>98.768807999999893</v>
+        <v>129.06806399999999</v>
       </c>
       <c r="E77">
         <f xml:space="preserve"> D77 - D74</f>
-        <v>1.1133359999999897</v>
+        <v>0.46990800000000377</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -8043,7 +8044,7 @@
         <v>14</v>
       </c>
       <c r="B78" s="1">
-        <v>97.655471999999904</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -8051,7 +8052,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="1">
-        <v>97.496424000000005</v>
+        <v>128.75479200000001</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>16</v>
@@ -8065,15 +8066,15 @@
         <v>14</v>
       </c>
       <c r="B80" s="1">
-        <v>98.768807999999893</v>
+        <v>129.06806399999999</v>
       </c>
       <c r="D80">
         <f>STDEV(B66:B95)</f>
-        <v>0.84589326890880312</v>
+        <v>5.1959647301839489</v>
       </c>
       <c r="E80">
         <f xml:space="preserve"> (D80 / E68) * 100</f>
-        <v>0.86101309276841576</v>
+        <v>4.087766556628182</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -8081,7 +8082,7 @@
         <v>14</v>
       </c>
       <c r="B81" s="1">
-        <v>98.132615999999999</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -8089,7 +8090,7 @@
         <v>14</v>
       </c>
       <c r="B82" s="1">
-        <v>98.927855999999906</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -8097,7 +8098,7 @@
         <v>14</v>
       </c>
       <c r="B83" s="1">
-        <v>98.450711999999996</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -8105,7 +8106,7 @@
         <v>14</v>
       </c>
       <c r="B84" s="1">
-        <v>97.973568</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -8113,7 +8114,7 @@
         <v>14</v>
       </c>
       <c r="B85" s="1">
-        <v>97.337375999999907</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -8121,7 +8122,7 @@
         <v>14</v>
       </c>
       <c r="B86" s="1">
-        <v>97.814520000000002</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -8129,7 +8130,7 @@
         <v>14</v>
       </c>
       <c r="B87" s="1">
-        <v>98.291663999999997</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -8137,7 +8138,7 @@
         <v>14</v>
       </c>
       <c r="B88" s="1">
-        <v>97.019279999999995</v>
+        <v>124.99552799999999</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -8145,7 +8146,7 @@
         <v>14</v>
       </c>
       <c r="B89" s="1">
-        <v>98.768807999999893</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -8153,7 +8154,7 @@
         <v>14</v>
       </c>
       <c r="B90" s="1">
-        <v>97.178327999999993</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -8161,7 +8162,7 @@
         <v>14</v>
       </c>
       <c r="B91" s="1">
-        <v>98.132615999999999</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -8169,7 +8170,7 @@
         <v>14</v>
       </c>
       <c r="B92" s="1">
-        <v>98.291663999999997</v>
+        <v>129.381336</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -8177,7 +8178,7 @@
         <v>14</v>
       </c>
       <c r="B93" s="1">
-        <v>99.086904000000004</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -8185,7 +8186,7 @@
         <v>14</v>
       </c>
       <c r="B94" s="1">
-        <v>96.224039999999903</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -8193,7 +8194,7 @@
         <v>14</v>
       </c>
       <c r="B95" s="1">
-        <v>98.132615999999999</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -8209,7 +8210,7 @@
         <v>10</v>
       </c>
       <c r="B98" s="1">
-        <v>95.335919999999902</v>
+        <v>111.14243999999999</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -8217,7 +8218,7 @@
         <v>10</v>
       </c>
       <c r="B99" s="1">
-        <v>96.437159999999906</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -8225,7 +8226,7 @@
         <v>10</v>
       </c>
       <c r="B100" s="1">
-        <v>95.965199999999996</v>
+        <v>128.13336000000001</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -8233,7 +8234,7 @@
         <v>10</v>
       </c>
       <c r="B101" s="1">
-        <v>95.335919999999902</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -8241,7 +8242,7 @@
         <v>10</v>
       </c>
       <c r="B102" s="1">
-        <v>96.279839999999993</v>
+        <v>127.50984</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -8249,7 +8250,7 @@
         <v>10</v>
       </c>
       <c r="B103" s="1">
-        <v>95.807879999999997</v>
+        <v>127.50984</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -8257,7 +8258,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="1">
-        <v>95.965199999999996</v>
+        <v>126.574559999999</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -8265,7 +8266,7 @@
         <v>10</v>
       </c>
       <c r="B105" s="1">
-        <v>95.021280000000004</v>
+        <v>127.50984</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -8273,7 +8274,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="1">
-        <v>96.279839999999993</v>
+        <v>126.88632</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -8281,7 +8282,7 @@
         <v>10</v>
       </c>
       <c r="B107" s="1">
-        <v>94.863960000000006</v>
+        <v>122.36579999999999</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -8289,7 +8290,7 @@
         <v>10</v>
       </c>
       <c r="B108" s="1">
-        <v>94.549319999999994</v>
+        <v>127.8216</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -8297,7 +8298,7 @@
         <v>10</v>
       </c>
       <c r="B109" s="1">
-        <v>95.807879999999997</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -8305,7 +8306,7 @@
         <v>10</v>
       </c>
       <c r="B110" s="1">
-        <v>95.49324</v>
+        <v>126.73044</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -8313,7 +8314,7 @@
         <v>10</v>
       </c>
       <c r="B111" s="1">
-        <v>95.178600000000003</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -8321,7 +8322,7 @@
         <v>10</v>
       </c>
       <c r="B112" s="1">
-        <v>95.49324</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -8329,7 +8330,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="1">
-        <v>95.807879999999997</v>
+        <v>126.418679999999</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -8337,7 +8338,7 @@
         <v>10</v>
       </c>
       <c r="B114" s="1">
-        <v>94.234679999999997</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -8345,7 +8346,7 @@
         <v>10</v>
       </c>
       <c r="B115" s="1">
-        <v>95.178600000000003</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -8353,7 +8354,7 @@
         <v>10</v>
       </c>
       <c r="B116" s="1">
-        <v>95.49324</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -8361,7 +8362,7 @@
         <v>10</v>
       </c>
       <c r="B117" s="1">
-        <v>95.021280000000004</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -8369,7 +8370,7 @@
         <v>10</v>
       </c>
       <c r="B118" s="1">
-        <v>95.335919999999902</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -8377,7 +8378,7 @@
         <v>10</v>
       </c>
       <c r="B119" s="1">
-        <v>95.021280000000004</v>
+        <v>127.97748</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -8385,7 +8386,7 @@
         <v>10</v>
       </c>
       <c r="B120" s="1">
-        <v>97.538399999999996</v>
+        <v>127.04219999999999</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -8393,7 +8394,7 @@
         <v>10</v>
       </c>
       <c r="B121" s="1">
-        <v>95.335919999999902</v>
+        <v>126.88632</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -8401,7 +8402,7 @@
         <v>10</v>
       </c>
       <c r="B122" s="1">
-        <v>95.807879999999997</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -8409,7 +8410,7 @@
         <v>10</v>
       </c>
       <c r="B123" s="1">
-        <v>95.178600000000003</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -8417,7 +8418,7 @@
         <v>10</v>
       </c>
       <c r="B124" s="1">
-        <v>95.178600000000003</v>
+        <v>121.898159999999</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -8425,7 +8426,7 @@
         <v>10</v>
       </c>
       <c r="B125" s="1">
-        <v>95.335919999999902</v>
+        <v>126.73044</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -8433,7 +8434,7 @@
         <v>10</v>
       </c>
       <c r="B126" s="1">
-        <v>95.335919999999902</v>
+        <v>127.35396</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -8441,7 +8442,7 @@
         <v>10</v>
       </c>
       <c r="B127" s="1">
-        <v>95.49324</v>
+        <v>127.19808</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -8449,7 +8450,7 @@
         <v>12</v>
       </c>
       <c r="B128" s="1">
-        <v>98.027315999999999</v>
+        <v>113.247828</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
@@ -8457,7 +8458,7 @@
         <v>12</v>
       </c>
       <c r="B129" s="1">
-        <v>99.452591999999996</v>
+        <v>132.04414800000001</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -8465,7 +8466,7 @@
         <v>12</v>
       </c>
       <c r="B130" s="1">
-        <v>98.502407999999903</v>
+        <v>115.91064</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -8473,7 +8474,7 @@
         <v>12</v>
       </c>
       <c r="B131" s="1">
-        <v>98.185680000000005</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -8481,7 +8482,7 @@
         <v>12</v>
       </c>
       <c r="B132" s="1">
-        <v>98.027315999999999</v>
+        <v>133.92377999999999</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -8489,7 +8490,7 @@
         <v>12</v>
       </c>
       <c r="B133" s="1">
-        <v>95.810220000000001</v>
+        <v>111.838104</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -8497,7 +8498,7 @@
         <v>12</v>
       </c>
       <c r="B134" s="1">
-        <v>98.344043999999997</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -8505,7 +8506,7 @@
         <v>12</v>
       </c>
       <c r="B135" s="1">
-        <v>97.235495999999898</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -8513,7 +8514,7 @@
         <v>12</v>
       </c>
       <c r="B136" s="1">
-        <v>96.918768</v>
+        <v>116.537184</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -8521,7 +8522,7 @@
         <v>12</v>
       </c>
       <c r="B137" s="1">
-        <v>97.393860000000004</v>
+        <v>133.45387199999999</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -8529,7 +8530,7 @@
         <v>12</v>
       </c>
       <c r="B138" s="1">
-        <v>97.393860000000004</v>
+        <v>116.380547999999</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -8537,7 +8538,7 @@
         <v>12</v>
       </c>
       <c r="B139" s="1">
-        <v>96.760403999999994</v>
+        <v>115.440732</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -8545,7 +8546,7 @@
         <v>12</v>
       </c>
       <c r="B140" s="1">
-        <v>98.502407999999903</v>
+        <v>133.297236</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -8553,7 +8554,7 @@
         <v>12</v>
       </c>
       <c r="B141" s="1">
-        <v>98.819136</v>
+        <v>133.297236</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -8561,7 +8562,7 @@
         <v>12</v>
       </c>
       <c r="B142" s="1">
-        <v>97.552223999999995</v>
+        <v>133.76714399999901</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -8569,7 +8570,7 @@
         <v>12</v>
       </c>
       <c r="B143" s="1">
-        <v>96.760403999999994</v>
+        <v>116.067275999999</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -8577,7 +8578,7 @@
         <v>12</v>
       </c>
       <c r="B144" s="1">
-        <v>96.918768</v>
+        <v>114.97082399999999</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -8585,7 +8586,7 @@
         <v>12</v>
       </c>
       <c r="B145" s="1">
-        <v>96.285312000000005</v>
+        <v>115.28409600000001</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -8593,7 +8594,7 @@
         <v>12</v>
       </c>
       <c r="B146" s="1">
-        <v>97.393860000000004</v>
+        <v>115.597368</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -8601,7 +8602,7 @@
         <v>12</v>
       </c>
       <c r="B147" s="1">
-        <v>97.235495999999898</v>
+        <v>118.260179999999</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -8609,7 +8610,7 @@
         <v>12</v>
       </c>
       <c r="B148" s="1">
-        <v>97.077131999999906</v>
+        <v>130.94769600000001</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -8617,7 +8618,7 @@
         <v>12</v>
       </c>
       <c r="B149" s="1">
-        <v>97.552223999999995</v>
+        <v>131.73087599999999</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -8625,7 +8626,7 @@
         <v>12</v>
       </c>
       <c r="B150" s="1">
-        <v>99.135863999999998</v>
+        <v>124.99552799999999</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -8633,7 +8634,7 @@
         <v>12</v>
       </c>
       <c r="B151" s="1">
-        <v>97.552223999999995</v>
+        <v>132.35741999999999</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -8641,7 +8642,7 @@
         <v>12</v>
       </c>
       <c r="B152" s="1">
-        <v>96.918768</v>
+        <v>131.41760399999899</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -8649,7 +8650,7 @@
         <v>12</v>
       </c>
       <c r="B153" s="1">
-        <v>98.185680000000005</v>
+        <v>131.26096799999999</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -8657,7 +8658,7 @@
         <v>12</v>
       </c>
       <c r="B154" s="1">
-        <v>96.918768</v>
+        <v>131.57424</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -8665,7 +8666,7 @@
         <v>12</v>
       </c>
       <c r="B155" s="1">
-        <v>96.443675999999996</v>
+        <v>131.41760399999899</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -8673,7 +8674,7 @@
         <v>12</v>
       </c>
       <c r="B156" s="1">
-        <v>98.977500000000006</v>
+        <v>131.88751199999999</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -8681,7 +8682,7 @@
         <v>12</v>
       </c>
       <c r="B157" s="1">
-        <v>96.760403999999994</v>
+        <v>134.863596</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
@@ -8689,7 +8690,7 @@
         <v>14</v>
       </c>
       <c r="B158" s="1">
-        <v>97.655471999999904</v>
+        <v>113.5611</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -8697,7 +8698,7 @@
         <v>14</v>
       </c>
       <c r="B159" s="1">
-        <v>98.768807999999893</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -8705,7 +8706,7 @@
         <v>14</v>
       </c>
       <c r="B160" s="1">
-        <v>99.405000000000001</v>
+        <v>111.211559999999</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -8713,7 +8714,7 @@
         <v>14</v>
       </c>
       <c r="B161" s="1">
-        <v>99.882143999999997</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -8721,7 +8722,7 @@
         <v>14</v>
       </c>
       <c r="B162" s="1">
-        <v>99.723095999999899</v>
+        <v>111.211559999999</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -8729,7 +8730,7 @@
         <v>14</v>
       </c>
       <c r="B163" s="1">
-        <v>97.655471999999904</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -8737,7 +8738,7 @@
         <v>14</v>
       </c>
       <c r="B164" s="1">
-        <v>98.927855999999906</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -8745,7 +8746,7 @@
         <v>14</v>
       </c>
       <c r="B165" s="1">
-        <v>98.768807999999893</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
@@ -8753,7 +8754,7 @@
         <v>14</v>
       </c>
       <c r="B166" s="1">
-        <v>99.245952000000003</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -8761,7 +8762,7 @@
         <v>14</v>
       </c>
       <c r="B167" s="1">
-        <v>97.337375999999907</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -8769,7 +8770,7 @@
         <v>14</v>
       </c>
       <c r="B168" s="1">
-        <v>97.655471999999904</v>
+        <v>129.85124399999901</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -8777,7 +8778,7 @@
         <v>14</v>
       </c>
       <c r="B169" s="1">
-        <v>98.609759999999994</v>
+        <v>128.28488399999901</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -8785,7 +8786,7 @@
         <v>14</v>
       </c>
       <c r="B170" s="1">
-        <v>97.655471999999904</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
@@ -8793,7 +8794,7 @@
         <v>14</v>
       </c>
       <c r="B171" s="1">
-        <v>97.496424000000005</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -8801,7 +8802,7 @@
         <v>14</v>
       </c>
       <c r="B172" s="1">
-        <v>98.768807999999893</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -8809,7 +8810,7 @@
         <v>14</v>
       </c>
       <c r="B173" s="1">
-        <v>98.132615999999999</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -8817,7 +8818,7 @@
         <v>14</v>
       </c>
       <c r="B174" s="1">
-        <v>98.927855999999906</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -8825,7 +8826,7 @@
         <v>14</v>
       </c>
       <c r="B175" s="1">
-        <v>98.450711999999996</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
@@ -8833,7 +8834,7 @@
         <v>14</v>
       </c>
       <c r="B176" s="1">
-        <v>97.973568</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -8841,7 +8842,7 @@
         <v>14</v>
       </c>
       <c r="B177" s="1">
-        <v>97.337375999999907</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -8849,7 +8850,7 @@
         <v>14</v>
       </c>
       <c r="B178" s="1">
-        <v>97.814520000000002</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -8857,7 +8858,7 @@
         <v>14</v>
       </c>
       <c r="B179" s="1">
-        <v>98.291663999999997</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
@@ -8865,7 +8866,7 @@
         <v>14</v>
       </c>
       <c r="B180" s="1">
-        <v>97.019279999999995</v>
+        <v>124.99552799999999</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -8873,7 +8874,7 @@
         <v>14</v>
       </c>
       <c r="B181" s="1">
-        <v>98.768807999999893</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
@@ -8881,7 +8882,7 @@
         <v>14</v>
       </c>
       <c r="B182" s="1">
-        <v>97.178327999999993</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -8889,7 +8890,7 @@
         <v>14</v>
       </c>
       <c r="B183" s="1">
-        <v>98.132615999999999</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -8897,7 +8898,7 @@
         <v>14</v>
       </c>
       <c r="B184" s="1">
-        <v>98.291663999999997</v>
+        <v>129.381336</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -8905,7 +8906,7 @@
         <v>14</v>
       </c>
       <c r="B185" s="1">
-        <v>99.086904000000004</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -8913,7 +8914,7 @@
         <v>14</v>
       </c>
       <c r="B186" s="1">
-        <v>96.224039999999903</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -8921,7 +8922,7 @@
         <v>14</v>
       </c>
       <c r="B187" s="1">
-        <v>98.132615999999999</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>